<commit_message>
add vis for eva and collect free text annotation grouped by criteria
</commit_message>
<xml_diff>
--- a/presentation/evavalues/avgscoreallgroups.xlsx
+++ b/presentation/evavalues/avgscoreallgroups.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git repositories\Auto_TextSum\presentation\evavalues\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE95A74A-C132-4277-8C6D-CA6C296D4E07}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F16BEA1B-F090-4B4F-AD38-69394FF52239}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -644,11 +644,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -699,6 +699,8 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFFFA500"/>
+      <color rgb="FF0000FF"/>
       <color rgb="FF9C1C1C"/>
     </mruColors>
   </colors>
@@ -1456,7 +1458,63 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:autoTitleDeleted val="1"/>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="de-DE" sz="1600" b="0" i="0" u="none" strike="noStrike" baseline="0"/>
+              <a:t>statistical Score Values over all Topics per Group</a:t>
+            </a:r>
+            <a:endParaRPr lang="de-DE" sz="1600"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="de-DE"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:barChart>
@@ -1660,10 +1718,7 @@
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="accent1">
-                <a:lumMod val="60000"/>
-                <a:lumOff val="40000"/>
-              </a:schemeClr>
+              <a:srgbClr val="FFA500"/>
             </a:solidFill>
             <a:ln w="19050">
               <a:solidFill>
@@ -1679,10 +1734,7 @@
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent1">
-                  <a:lumMod val="60000"/>
-                  <a:lumOff val="40000"/>
-                </a:schemeClr>
+                <a:srgbClr val="FFA500"/>
               </a:solidFill>
               <a:ln w="19050">
                 <a:solidFill>
@@ -1703,7 +1755,7 @@
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="9C1C1C"/>
+                <a:srgbClr val="0000FF"/>
               </a:solidFill>
               <a:ln w="19050">
                 <a:solidFill>
@@ -1793,10 +1845,7 @@
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="accent1">
-                <a:lumMod val="60000"/>
-                <a:lumOff val="40000"/>
-              </a:schemeClr>
+              <a:srgbClr val="FFA500"/>
             </a:solidFill>
             <a:ln w="19050">
               <a:solidFill>
@@ -1812,10 +1861,7 @@
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent1">
-                  <a:lumMod val="60000"/>
-                  <a:lumOff val="40000"/>
-                </a:schemeClr>
+                <a:srgbClr val="FFA500"/>
               </a:solidFill>
               <a:ln w="19050">
                 <a:solidFill>
@@ -1836,7 +1882,7 @@
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="9C1C1C"/>
+                <a:srgbClr val="0000FF"/>
               </a:solidFill>
               <a:ln w="19050">
                 <a:solidFill>
@@ -2196,7 +2242,9 @@
       <a:schemeClr val="bg1"/>
     </a:solidFill>
     <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:noFill/>
+      <a:solidFill>
+        <a:schemeClr val="tx1"/>
+      </a:solidFill>
       <a:round/>
     </a:ln>
     <a:effectLst/>
@@ -2213,8 +2261,8 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.78740157499999996" l="0.7" r="0.7" t="0.78740157499999996" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup paperSize="9" orientation="landscape"/>
   </c:printSettings>
 </c:chartSpace>
 </file>
@@ -3270,7 +3318,63 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:autoTitleDeleted val="1"/>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="de-DE" sz="1600" b="0" i="0" u="none" strike="noStrike" baseline="0"/>
+              <a:t>calculated Score per Topic</a:t>
+            </a:r>
+            <a:endParaRPr lang="de-DE" sz="1600"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="de-DE"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:lineChart>
@@ -3293,10 +3397,7 @@
           <c:spPr>
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent1">
-                  <a:lumMod val="60000"/>
-                  <a:lumOff val="40000"/>
-                </a:schemeClr>
+                <a:srgbClr val="FFA500"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -3641,7 +3742,7 @@
           <c:spPr>
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
-                <a:srgbClr val="9C1C1C"/>
+                <a:srgbClr val="0000FF"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -4079,7 +4180,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -4270,7 +4371,9 @@
       <a:schemeClr val="bg1"/>
     </a:solidFill>
     <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:noFill/>
+      <a:solidFill>
+        <a:schemeClr val="tx1"/>
+      </a:solidFill>
       <a:round/>
     </a:ln>
     <a:effectLst/>
@@ -4287,8 +4390,8 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.78740157499999996" l="0.7" r="0.7" t="0.78740157499999996" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup paperSize="9" orientation="landscape"/>
   </c:printSettings>
 </c:chartSpace>
 </file>
@@ -5211,7 +5314,67 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:autoTitleDeleted val="1"/>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="de-DE" sz="1600"/>
+              <a:t>calculated Score</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="de-DE" sz="1600" baseline="0"/>
+              <a:t> per Topic - sorted</a:t>
+            </a:r>
+            <a:endParaRPr lang="de-DE" sz="1600"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="de-DE"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:lineChart>
@@ -5234,10 +5397,7 @@
           <c:spPr>
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent1">
-                  <a:lumMod val="60000"/>
-                  <a:lumOff val="40000"/>
-                </a:schemeClr>
+                <a:srgbClr val="FFA500"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -5440,7 +5600,7 @@
           <c:spPr>
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
-                <a:srgbClr val="9C1C1C"/>
+                <a:srgbClr val="0000FF"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -5645,69 +5805,6 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US" sz="1100"/>
-                  <a:t>sorted</a:t>
-                </a:r>
-                <a:r>
-                  <a:rPr lang="en-US" sz="1100" baseline="0"/>
-                  <a:t> </a:t>
-                </a:r>
-                <a:r>
-                  <a:rPr lang="en-US" sz="1100"/>
-                  <a:t>evaluated summaries</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="de-DE"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
@@ -5874,6 +5971,16 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="tr"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.88009942129629637"/>
+          <c:y val="0.79236828703703688"/>
+          <c:w val="9.7851967592592598E-2"/>
+          <c:h val="0.11345138888888889"/>
+        </c:manualLayout>
+      </c:layout>
       <c:overlay val="1"/>
       <c:spPr>
         <a:solidFill>
@@ -5889,7 +5996,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1050" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+            <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -5922,10 +6029,7 @@
     </a:solidFill>
     <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
       <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
+        <a:schemeClr val="tx1"/>
       </a:solidFill>
       <a:round/>
     </a:ln>
@@ -5943,8 +6047,8 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.78740157499999996" l="0.7" r="0.7" t="0.78740157499999996" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup paperSize="9" orientation="landscape"/>
   </c:printSettings>
 </c:chartSpace>
 </file>
@@ -9291,15 +9395,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>478846</xdr:colOff>
-      <xdr:row>49</xdr:row>
-      <xdr:rowOff>80091</xdr:rowOff>
+      <xdr:colOff>680552</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>158532</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>710864</xdr:colOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>176552</xdr:colOff>
       <xdr:row>78</xdr:row>
-      <xdr:rowOff>91423</xdr:rowOff>
+      <xdr:rowOff>97032</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -9328,16 +9432,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>51</xdr:col>
-      <xdr:colOff>170293</xdr:colOff>
-      <xdr:row>74</xdr:row>
-      <xdr:rowOff>3605</xdr:rowOff>
+      <xdr:col>36</xdr:col>
+      <xdr:colOff>672519</xdr:colOff>
+      <xdr:row>81</xdr:row>
+      <xdr:rowOff>142150</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>66</xdr:col>
-      <xdr:colOff>368293</xdr:colOff>
-      <xdr:row>103</xdr:row>
-      <xdr:rowOff>44705</xdr:rowOff>
+      <xdr:col>52</xdr:col>
+      <xdr:colOff>108519</xdr:colOff>
+      <xdr:row>110</xdr:row>
+      <xdr:rowOff>183250</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -9364,16 +9468,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>275646</xdr:colOff>
-      <xdr:row>49</xdr:row>
-      <xdr:rowOff>129163</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>414191</xdr:colOff>
+      <xdr:row>56</xdr:row>
+      <xdr:rowOff>77209</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>32</xdr:col>
-      <xdr:colOff>473646</xdr:colOff>
-      <xdr:row>78</xdr:row>
-      <xdr:rowOff>170263</xdr:rowOff>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>672191</xdr:colOff>
+      <xdr:row>79</xdr:row>
+      <xdr:rowOff>15709</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -9441,16 +9545,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>733424</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>66674</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>180974</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>57149</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
-      <xdr:colOff>169424</xdr:colOff>
-      <xdr:row>36</xdr:row>
-      <xdr:rowOff>143774</xdr:rowOff>
+      <xdr:colOff>438974</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>186149</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -9777,8 +9881,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BB48"/>
   <sheetViews>
-    <sheetView topLeftCell="A39" zoomScale="84" workbookViewId="0">
-      <selection activeCell="Q64" sqref="Q64"/>
+    <sheetView zoomScale="25" zoomScaleNormal="25" workbookViewId="0">
+      <selection activeCell="AB78" sqref="AB78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10122,7 +10226,7 @@
         <v>4.4417755704735704</v>
       </c>
       <c r="B4" s="1">
-        <f t="shared" ref="B4:B20" si="1">INDEX($F3:$BB3, MATCH(A4,$F4:$BB4,0))</f>
+        <f t="shared" ref="B4:B19" si="1">INDEX($F3:$BB3, MATCH(A4,$F4:$BB4,0))</f>
         <v>4.4275519421860903</v>
       </c>
       <c r="C4" s="1">
@@ -10130,7 +10234,7 @@
         <v>2.2487604343187102</v>
       </c>
       <c r="D4" s="4">
-        <f t="shared" ref="D4:D20" si="3">INDEX($F3:$BB3, MATCH(C4,$F4:$BB4,0))</f>
+        <f t="shared" ref="D4:D19" si="3">INDEX($F3:$BB3, MATCH(C4,$F4:$BB4,0))</f>
         <v>2.3055555555555598</v>
       </c>
       <c r="E4" s="1" t="s">
@@ -13795,25 +13899,25 @@
       </c>
     </row>
     <row r="33" spans="4:17" x14ac:dyDescent="0.25">
-      <c r="D33" s="6"/>
+      <c r="D33" s="5"/>
     </row>
     <row r="34" spans="4:17" x14ac:dyDescent="0.25">
-      <c r="E34" s="5" t="s">
+      <c r="E34" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="F34" s="5"/>
-      <c r="G34" s="5"/>
-      <c r="H34" s="5"/>
-      <c r="I34" s="5"/>
-      <c r="J34" s="5"/>
-      <c r="L34" s="5" t="s">
+      <c r="F34" s="6"/>
+      <c r="G34" s="6"/>
+      <c r="H34" s="6"/>
+      <c r="I34" s="6"/>
+      <c r="J34" s="6"/>
+      <c r="L34" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="M34" s="5"/>
-      <c r="N34" s="5"/>
-      <c r="O34" s="5"/>
-      <c r="P34" s="5"/>
-      <c r="Q34" s="5"/>
+      <c r="M34" s="6"/>
+      <c r="N34" s="6"/>
+      <c r="O34" s="6"/>
+      <c r="P34" s="6"/>
+      <c r="Q34" s="6"/>
     </row>
     <row r="35" spans="4:17" x14ac:dyDescent="0.25">
       <c r="E35" s="2" t="s">
@@ -14187,7 +14291,7 @@
         <v>2.3018575851393202</v>
       </c>
       <c r="G44" s="1">
-        <f t="shared" ref="G44:K44" si="21">G36</f>
+        <f t="shared" ref="G44:J44" si="21">G36</f>
         <v>2.6516057585824999</v>
       </c>
       <c r="H44" s="1">
@@ -14211,7 +14315,7 @@
         <v>2.2487604343187102</v>
       </c>
       <c r="N44" s="1">
-        <f t="shared" ref="N44:R48" si="23">N36</f>
+        <f t="shared" ref="N44:P44" si="23">N36</f>
         <v>2.6087598675833998</v>
       </c>
       <c r="O44" s="1">
@@ -14454,8 +14558,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23762BC7-8DEB-4B59-8C47-55F9E118F12F}">
   <dimension ref="A1:AX59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="T17" sqref="T17"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="P35" sqref="P35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16427,6 +16531,7 @@
     <sortCondition ref="D10"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
unified layout for dia
</commit_message>
<xml_diff>
--- a/presentation/evavalues/avgscoreallgroups.xlsx
+++ b/presentation/evavalues/avgscoreallgroups.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git repositories\Auto_TextSum\presentation\evavalues\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F16BEA1B-F090-4B4F-AD38-69394FF52239}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC0FB863-AFB1-4982-A07D-B129AAE72078}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20400" windowHeight="7545" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="avgscoreallgroups" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="37">
   <si>
     <t>Gruppe1</t>
   </si>
@@ -111,12 +111,6 @@
   </si>
   <si>
     <t>Group 6</t>
-  </si>
-  <si>
-    <t>Score</t>
-  </si>
-  <si>
-    <t>Ø Score per Topic</t>
   </si>
   <si>
     <t>g5</t>
@@ -2149,7 +2143,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Score</c:v>
+                  <c:v>score</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3389,7 +3383,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Ø Score per Topic</c:v>
+                  <c:v>Average</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -4124,7 +4118,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US" sz="1100"/>
-                  <a:t>Topic</a:t>
+                  <a:t>topic</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -4245,7 +4239,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US" sz="1100"/>
-                  <a:t>Score</a:t>
+                  <a:t>score</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -5892,7 +5886,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US" sz="1100"/>
-                  <a:t>Score</a:t>
+                  <a:t>score</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -5975,7 +5969,7 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.88009942129629637"/>
+          <c:x val="0.88891886574074086"/>
           <c:y val="0.79236828703703688"/>
           <c:w val="9.7851967592592598E-2"/>
           <c:h val="0.11345138888888889"/>
@@ -9881,8 +9875,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BB48"/>
   <sheetViews>
-    <sheetView zoomScale="25" zoomScaleNormal="25" workbookViewId="0">
-      <selection activeCell="AB78" sqref="AB78"/>
+    <sheetView tabSelected="1" topLeftCell="M55" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B56" sqref="B56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13482,7 +13476,7 @@
         <v>1019</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="F31" s="1">
         <f t="shared" ref="F31:AK31" si="11">AVERAGE(F4,F8,F12,F16,F20)</f>
@@ -13911,7 +13905,7 @@
       <c r="I34" s="6"/>
       <c r="J34" s="6"/>
       <c r="L34" s="6" t="s">
-        <v>30</v>
+        <v>1</v>
       </c>
       <c r="M34" s="6"/>
       <c r="N34" s="6"/>
@@ -14558,15 +14552,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23762BC7-8DEB-4B59-8C47-55F9E118F12F}">
   <dimension ref="A1:AX59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="P35" sqref="P35"/>
+    <sheetView topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K38" sqref="K38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B1">
         <v>3.836999716162238</v>
@@ -14718,7 +14712,7 @@
     </row>
     <row r="2" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B2">
         <v>3.6209684633051502</v>
@@ -14870,7 +14864,7 @@
     </row>
     <row r="3" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B3">
         <v>3.3240369579716802</v>
@@ -15022,7 +15016,7 @@
     </row>
     <row r="4" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B4">
         <v>3.9169435215946802</v>
@@ -15174,7 +15168,7 @@
     </row>
     <row r="5" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B5" s="1">
         <v>4.3995431339291002</v>
@@ -15320,7 +15314,7 @@
     </row>
     <row r="6" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B6" s="1">
         <v>3.9235065040105801</v>
@@ -15481,22 +15475,22 @@
     </row>
     <row r="10" spans="1:50" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C10" t="s">
         <v>28</v>
       </c>
       <c r="D10" t="s">
+        <v>32</v>
+      </c>
+      <c r="E10" t="s">
+        <v>33</v>
+      </c>
+      <c r="F10" t="s">
         <v>34</v>
       </c>
-      <c r="E10" t="s">
+      <c r="G10" t="s">
         <v>35</v>
-      </c>
-      <c r="F10" t="s">
-        <v>36</v>
-      </c>
-      <c r="G10" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="11" spans="1:50" x14ac:dyDescent="0.25">

</xml_diff>